<commit_message>
added xpulp v2 verif plan
- Added v2 plans for xpulp instructions set. Except HWloop, all plans are not standalone and are dependent to formal verification
- For legacy concerns, old verif plans for v1 have been moved at then end of the v2 files
- added back previously deleted xpulp_postinc Vplan
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmcconnell\Desktop\CV32E40P VPLANS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/Verification/v2_VerifPlans/Simulation/instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_8CED7AB55E2ADA2A22687483D34082A05C1D0B07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C59ACAA-F0EE-4FC1-B82C-D31C4EF93895}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -200,13 +201,22 @@
   </si>
   <si>
     <t>Test random values of ls3 with all valid values of ls2 (0, 1, 2)</t>
+  </si>
+  <si>
+    <t>Link to Coverage</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Below are plans for CV32E40P v1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,13 +239,41 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -251,7 +289,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -262,14 +300,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -282,6 +344,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -546,14 +612,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:XFD24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
     <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
@@ -566,252 +632,149 @@
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9 16384:16384" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="60">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="I1" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="XFD2" s="2"/>
+    </row>
+    <row r="3" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="I6" s="13"/>
+    </row>
+    <row r="7" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="I7" s="13"/>
+    </row>
+    <row r="8" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="11"/>
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="60">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="60">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="60">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="60" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>43</v>
@@ -826,7 +789,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="45">
+    <row r="11" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -834,10 +797,10 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>34</v>
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
@@ -852,7 +815,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="45">
+    <row r="12" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -860,155 +823,604 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9 16384:16384" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9 16384:16384" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9 16384:16384" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9 16384:16384" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="60">
-      <c r="A13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="45">
-      <c r="A14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="F20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" t="s">
+        <v>40</v>
+      </c>
+      <c r="H20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G14" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45">
-      <c r="A15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="F21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D22" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F15" t="s">
-        <v>41</v>
-      </c>
-      <c r="G15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45">
-      <c r="A16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="F22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G22" t="s">
+        <v>40</v>
+      </c>
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F16" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
-      <c r="H16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="75">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" t="s">
+        <v>40</v>
+      </c>
+      <c r="H23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F17" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6f429ff05de3a495de36a912eeee1367">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dba9ee4a9862521e056f2186065b8ec" ns2:_="" ns3:_="">
+    <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <xsd:import namespace="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="68bd86b6-d639-4884-9680-62e746fab3da" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="21" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="51aa521f-7cbd-47c5-afee-4a8147a04eed" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{67132edb-7ad2-4046-b569-46a3488a100c}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="51aa521f-7cbd-47c5-afee-4a8147a04eed">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Type de contenu"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titre"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0813D6E-6704-44BB-86A0-53EB7147135C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E67A2DEA-627F-45CD-8A5E-DEB4B7BB5A7D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
+    <ds:schemaRef ds:uri="51aa521f-7cbd-47c5-afee-4a8147a04eed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
first batch of updates to xpulp vplans
Coverage items for non-initially planned instructions (verified in formal) have been added as random instruction generator will generate all xpulp instructions anyway, including these.
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dolphinintegrationfr.sharepoint.com/sites/PANTHER/Documents partages/General/CV32E40P/Verification/v2_VerifPlans/Simulation/instructions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\corev-v-verif\cv32e40p\docs\VerifPlans\Simulation\xpulp_instruction_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_8CED7AB55E2ADA2A22687483D34082A05C1D0B07" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C59ACAA-F0EE-4FC1-B82C-D31C4EF93895}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0C17B3-12A2-4CEC-8EB8-9F6E60DA49E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="3705" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="109">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -206,10 +217,269 @@
     <t>Link to Coverage</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Below are plans for CV32E40P v1</t>
+  </si>
+  <si>
+    <t>CV32E40P User Manual - Chapter 17.4.2 Bit Manipulation operations</t>
+  </si>
+  <si>
+    <t>RV32Xpulp Bit Manipulation operations</t>
+  </si>
+  <si>
+    <t>CV.EXTRACT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register operands 
+All possible rs1 registers are used.
+All possible rs2 registers are used.
+All possible rD registers are used.
+All possible register combinations where first operand is the destination register of the previous instruction  
+All possible register combinations where second operand is the destination register of the previous instruction
+</t>
+  </si>
+  <si>
+    <t>Check against RM</t>
+  </si>
+  <si>
+    <t>Constrained-Random</t>
+  </si>
+  <si>
+    <t>Functional Coverage</t>
+  </si>
+  <si>
+    <t>coverage:
+All bits of rs1 are toggled 
+All bits of Is2 are toggled 
+All bits of Is3 are toggled 
+All bits of rD are toggled</t>
+  </si>
+  <si>
+    <t>CV.EXTRACTU</t>
+  </si>
+  <si>
+    <t>CV.EXTRACTR</t>
+  </si>
+  <si>
+    <t>CV.EXTRACTUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register operands 
+All possible rs1 registers are used.
+All possible rD registers are used.
+All possible register combinations where first operand is the destination register of the previous instruction  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register operands 
+All possible rs1 registers are used.
+All possible rD registers are used.
+All possible register combinations where first operand is the destination register of the previous instruction </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register operands 
+All possible rs1 registers are used.
+All possible rD registers are used.
+All possible register combinations where first operand is the destination register of the previous instruction  </t>
+  </si>
+  <si>
+    <t>coverage:
+All bits of rs1 are toggled 
+bits rs2[9:0] are toggled 
+All bits of rD are toggled</t>
+  </si>
+  <si>
+    <t>coverage:
+All bits of rs1 are toggled 
+bits rs2[9:0] are toggled  
+All bits of rD are toggled</t>
+  </si>
+  <si>
+    <t>CV.INSERT</t>
+  </si>
+  <si>
+    <t>cv.insert rD, rs1, Is3, Is2 
+rD[min(Is3+Is2,31):Is2] = rs1[Is3-(max(Is3+Is2,31)-31):0]
+The rest of the bits of rD are untouched and keep their previous value.
+Is3 + Is2 must be &lt; 32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv.extractur rD, rs1, rs2
+rD = Zext(rs1[min(rs2[9:5]+rs2[4:0],31):rs2[4:0]])
+</t>
+  </si>
+  <si>
+    <t>cv.extractr rD, rs1, rs2
+rD = Sext(rs1[min(rs2[9:5]+rs2[4:0],31):rs2[4:0]])
+Note: Sign extension is done over the MSB of the extracted part.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cv.extractu rD, rs1, Is3, Is2 
+rD = Zext(rs1[min(Is3+Is2,31):Is2])
+</t>
+  </si>
+  <si>
+    <t>cv.extract rD, rs1, Is3, Is2 
+rD = Sext(rs1[min(Is3+Is2,31):Is2])
+Note: Sign extension is done over the MSB of the extracted part.</t>
+  </si>
+  <si>
+    <t>CV.INSERTR</t>
+  </si>
+  <si>
+    <t>cv.insert rD, rs1, rs2
+rD[min(rs2[9:5]+rs2[4:0],31):rs2[4:0]] =
+rs1[rs2[9:5]-(max(rs2[9:5]+rs2[4:0],31)-31):0]
+The rest of the bits of rD are untouched and keep their previous value.
+rs2[9:5]+rs2[4:0] must be &lt; 32</t>
+  </si>
+  <si>
+    <t>CV.BCLR</t>
+  </si>
+  <si>
+    <t>CV.BCLRR</t>
+  </si>
+  <si>
+    <t>cv.bclr rD, rs1, Is3, Is2 
+rD[min(Is3+Is2,31):Is2] bits set to 0
+The rest of the bits of rD are passed through from rs1 and are not modified.</t>
+  </si>
+  <si>
+    <t>cv.bclrr rD, rs1, rs2 
+rD[min(rs2[9:5]+rs2[4:0],31):rs2[4:0]] bits set to 0
+The rest of the bits of rD are passed through from rs1 and are not modified.</t>
+  </si>
+  <si>
+    <t>Input Values:
+Is2 is 0, 31, any other value
+Is3 is 0, 31, any other value
+rs1 is -ve, +ve, 0
+rs1[min(Is3+Is2,31)] is 0, 1</t>
+  </si>
+  <si>
+    <t>Input Values:
+Is2 is 0, 31, any other value
+Is3 is 0, 31, any other value
+rs1 is +ve, 0</t>
+  </si>
+  <si>
+    <t>Input Values:
+rs2[4:0] is 0, 31, any other value
+rs2[9:5] is 0, 31, any other value
+rs1 is -ve, +ve, 0
+rs1[min(rs2[9:5]+rs2[4:0],31)] is 0, 1</t>
+  </si>
+  <si>
+    <t>Input Values:
+rs2[4:0] is 0, 31, any other value
+rs2[9:5] is 0, 31, any other value
+rs1 is +ve, 0</t>
+  </si>
+  <si>
+    <t>CV.BSET</t>
+  </si>
+  <si>
+    <t>cv.bset rD, rs1, Is3, Is2 
+rD[min(Is3+Is2,31):Is2] bits set to 1
+The rest of the bits of rD are passed through from rs1 and are not modified.</t>
+  </si>
+  <si>
+    <t>CV.BSETR</t>
+  </si>
+  <si>
+    <t>cv.bsetr rD, rs1, rs2
+ rD[min(rs2[9:5]+rs2[4:0],31):rs2[4:0]] bits set to 1
+The rest of the bits of rD are passed through from rs1 and are not modified.</t>
+  </si>
+  <si>
+    <t>CV.FF1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Register operands 
+All possible rs1 registers are used.
+All possible rD registers are used.
+All possible register combinations where first operand is the destination register of the previous instruction  
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coverage:
+All bits of rs1 are toggled 
+</t>
+  </si>
+  <si>
+    <t>CV.FL1</t>
+  </si>
+  <si>
+    <t>Input Values:
+rs1 is 0, 32'h8000_0001, 32'h8000_0000, 1</t>
+  </si>
+  <si>
+    <t>Input Values:
+rs1 is 0, 32'h8000_0001, 1, 32'h8000_0000,</t>
+  </si>
+  <si>
+    <t>CV.CLB</t>
+  </si>
+  <si>
+    <t>cv.clb rD, rs1 
+rD = count leading bits of rs1
+Number of consecutive 1’s or 0’s starting from MSB.
+If rs1 is 0, rD will be 0. If rs1 is different than 0, returns (number - 1)</t>
+  </si>
+  <si>
+    <t>cv.ff1 rD, rs1 
+rD = bit position of the first bit set in rs1, starting from LSB.
+If bit 0 is set, rD will be 0. If only bit 31 is set, rD will be 31.
+If rs1 is 0, rD will be 32.</t>
+  </si>
+  <si>
+    <t>cv.fl1 rD, rs1 
+rD = bit position of the last bit set in rs1, starting from LSB.
+If only bit 0 is set, rD will be 0. If bit 31 is set, rD will be 31.
+If rs1 is 0, rD will be 32.</t>
+  </si>
+  <si>
+    <t>Input Values:
+rs1 is +ve, 0, -1, -ve</t>
+  </si>
+  <si>
+    <t>coverage:
+All bits of rs1 are toggled 
+All bits of rD are toggled</t>
+  </si>
+  <si>
+    <t>CV.CNT</t>
+  </si>
+  <si>
+    <t>cv.cnt rD, rs1 
+rD = Population count of rs1
+Number of bits set in rs1</t>
+  </si>
+  <si>
+    <t>cv.ror rD, rs1, rs2 
+rD = RotateRight(rs1, rs2)</t>
+  </si>
+  <si>
+    <t>CV.ROR</t>
+  </si>
+  <si>
+    <t>Input Values:
+rs2 is 0, 1, 32, any other value</t>
+  </si>
+  <si>
+    <t>CV.BITREV</t>
+  </si>
+  <si>
+    <t>cv.bitrev rD, rs1, Is3, Is2 
+Given an input rs1 it returns a bit reversed representation assuming
+FFT on 2^Is2 points in Radix 2^(Is3+1).
+Is3 can be either 0 (radix-2), 1 (radix-4) or 2 (radix-8).
+Note: When Is3 = 3, instruction has the same bahavior as if it was 0 (radix-2)</t>
+  </si>
+  <si>
+    <t>Input Values:
+Is2 is 0, 31, any other value
+Is3 is 0, 31, any other value
+rs1 is -ve, +ve, 0</t>
   </si>
 </sst>
 </file>
@@ -289,18 +559,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -328,6 +591,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -344,10 +637,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -613,561 +902,1465 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD24"/>
+  <dimension ref="A1:XFD73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.28515625" customWidth="1"/>
-    <col min="5" max="5" width="41.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" style="16" customWidth="1"/>
     <col min="6" max="6" width="21.7109375" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.85546875" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9 16384:16384" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:9 16384:16384" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:9 16384:16384" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="XFD2" s="1"/>
+    </row>
+    <row r="3" spans="1:9 16384:16384" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9 16384:16384" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9 16384:16384" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9 16384:16384" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9 16384:16384" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="18"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9 16384:16384" ht="180" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9 16384:16384" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9 16384:16384" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9 16384:16384" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9 16384:16384" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9 16384:16384" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9 16384:16384" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9 16384:16384" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9 16384:16384" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="18"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="18"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="18"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A29" s="18"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="18"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A32" s="18"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="18"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="18"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="18"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="18"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="18"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="18"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H40" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="18"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="F41" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H41" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F43" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H43" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F44" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H44" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="18"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F45" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H45" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F46" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H46" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H47" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="18"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="8"/>
+      <c r="D55" s="13"/>
+      <c r="I55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="XFD2" s="2"/>
-    </row>
-    <row r="3" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:9 16384:16384" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="I6" s="13"/>
-    </row>
-    <row r="7" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="I7" s="13"/>
-    </row>
-    <row r="8" spans="1:9 16384:16384" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="I8" s="13"/>
-    </row>
-    <row r="9" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B56" s="8"/>
+      <c r="D56" s="13"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+      <c r="D57" s="13"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B58" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C58" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D58" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E58" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F58" t="s">
         <v>41</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G58" t="s">
         <v>40</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="59" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B59" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C59" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D59" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E59" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F59" t="s">
         <v>41</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G59" t="s">
         <v>40</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B60" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C60" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D60" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E60" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F60" t="s">
         <v>41</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G60" t="s">
         <v>40</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H60" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:9 16384:16384" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="61" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A61" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B61" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C61" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D61" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E61" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F61" t="s">
         <v>41</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G61" t="s">
         <v>40</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H61" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9 16384:16384" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+    <row r="62" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B62" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C62" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D62" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E62" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F62" t="s">
         <v>41</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G62" t="s">
         <v>40</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H62" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:9 16384:16384" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="63" spans="1:9" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B63" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C63" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D63" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E63" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F63" t="s">
         <v>41</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G63" t="s">
         <v>40</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H63" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9 16384:16384" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="64" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B64" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C64" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D64" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E64" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F64" t="s">
         <v>41</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G64" t="s">
         <v>40</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H64" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:9 16384:16384" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B65" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C65" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D65" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E65" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F65" t="s">
         <v>41</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G65" t="s">
         <v>40</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H65" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B66" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C66" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D66" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E66" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F66" t="s">
         <v>41</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G66" t="s">
         <v>40</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H66" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B67" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C67" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D67" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E67" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F67" t="s">
         <v>41</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G67" t="s">
         <v>40</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H67" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="68" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B68" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C68" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D68" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E68" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F68" t="s">
         <v>41</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G68" t="s">
         <v>40</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H68" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="69" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B69" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C69" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D69" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E69" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F69" t="s">
         <v>41</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G69" t="s">
         <v>40</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H69" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+    <row r="70" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B70" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C70" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D70" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E70" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F70" t="s">
         <v>41</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G70" t="s">
         <v>40</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H70" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+    <row r="71" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B71" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C71" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D71" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E71" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F71" t="s">
         <v>41</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G71" t="s">
         <v>40</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H71" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B72" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C72" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D72" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E72" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F72" t="s">
         <v>41</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G72" t="s">
         <v>40</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H72" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+    <row r="73" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B73" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C73" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D73" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="E73" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F73" t="s">
         <v>41</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G73" t="s">
         <v>40</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H73" t="s">
         <v>42</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="34">
+    <mergeCell ref="B2:B49"/>
+    <mergeCell ref="A2:A49"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6f429ff05de3a495de36a912eeee1367">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dba9ee4a9862521e056f2186065b8ec" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -1398,15 +2591,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0813D6E-6704-44BB-86A0-53EB7147135C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E67A2DEA-627F-45CD-8A5E-DEB4B7BB5A7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1423,4 +2617,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0813D6E-6704-44BB-86A0-53EB7147135C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated columns with new info required by Mike & name changes
</commit_message>
<xml_diff>
--- a/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
+++ b/cv32e40p/docs/VerifPlans/Simulation/xpulp_instruction_extensions/CV32E40P_xpulp-bitmanipulations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Simulation - Copie\xpulp_instruction_extensions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git_repos\corev-v-verif\cv32e40p\docs\VerifPlans\Simulation\xpulp_instruction_extensions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB42D99C-EFE2-4099-A76F-47D19072235A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8921C726-0268-4230-8D8C-8CC8BF326091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="5250" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="178">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -469,9 +469,6 @@
 rs1 is +ve, 0, 1, -1, -ve</t>
   </si>
   <si>
-    <t>Related Test Program(s)</t>
-  </si>
-  <si>
     <t>corev_rand_pulp_instr_test
 pulp_bit_manipulation</t>
   </si>
@@ -790,6 +787,18 @@
     <t xml:space="preserve">Toggle is not a requirement of CV32E40Pv2 verification, but the corresponding coverage from the Reference Model Coverage Package exists and is given for reference purposes only
 Immediate toggle coverage is missing from Reference Model Coverage Package.
 </t>
+  </si>
+  <si>
+    <t>Test-Program Type</t>
+  </si>
+  <si>
+    <t>UMV Test Config</t>
+  </si>
+  <si>
+    <t>see CV32E40Pv2_test_list.xlsx</t>
+  </si>
+  <si>
+    <t>Test-Program(s) Name(s)</t>
   </si>
 </sst>
 </file>
@@ -869,7 +878,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -927,20 +936,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1237,17 +1243,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1258,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,15 +1277,16 @@
     <col min="3" max="3" width="23.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" style="16" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
     <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="86" customWidth="1"/>
-    <col min="11" max="11" width="67.7109375" style="12" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="86" customWidth="1"/>
+    <col min="12" max="12" width="67.7109375" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1295,1270 +1302,1481 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>106</v>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>174</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>175</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="B2" s="21" t="s">
+      <c r="L1" s="17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="22" t="s">
         <v>73</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>57</v>
+      <c r="F2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J2" s="13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="24"/>
+      <c r="J2" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="22"/>
       <c r="E3" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>57</v>
+      <c r="F3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="12" t="s">
-        <v>112</v>
+      <c r="J3" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="24"/>
+        <v>111</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="24"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="22"/>
       <c r="E4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>57</v>
+      <c r="F4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J4" s="12" t="s">
-        <v>113</v>
+      <c r="J4" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K4" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="22" t="s">
         <v>72</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>57</v>
+      <c r="F5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J5" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="21"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="24"/>
+      <c r="J5" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="22"/>
       <c r="E6" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>57</v>
+      <c r="F6" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I6" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J6" s="12" t="s">
-        <v>115</v>
+      <c r="J6" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="24"/>
+        <v>114</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="22"/>
       <c r="E7" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>57</v>
+      <c r="F7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>116</v>
+      <c r="J7" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K7" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A8" s="21"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="22" t="s">
         <v>71</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F8" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>57</v>
+      <c r="F8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="J8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="24"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="12" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="24"/>
+    <row r="10" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>57</v>
+      <c r="F10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="12" t="s">
-        <v>119</v>
+      <c r="J10" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="L10" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="22" t="s">
         <v>70</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F11" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>57</v>
+      <c r="F11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="24"/>
+      <c r="J11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="25"/>
-      <c r="G12" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>57</v>
+      <c r="F12" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J12" s="12" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="24"/>
+      <c r="J12" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="25"/>
-      <c r="G13" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>57</v>
+      <c r="F13" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="12" t="s">
-        <v>119</v>
+      <c r="J13" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="21" t="s">
         <v>69</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>57</v>
+      <c r="F14" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="J14" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>57</v>
+      <c r="F15" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I15" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J15" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+      <c r="J15" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="21"/>
       <c r="E16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>57</v>
+      <c r="F16" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J16" s="12" t="s">
-        <v>123</v>
+      <c r="J16" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K16" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A17" s="21"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="21" t="s">
         <v>104</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>57</v>
+      <c r="F17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I17" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J17" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="21"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="23"/>
+      <c r="J17" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="21"/>
       <c r="E18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>57</v>
+      <c r="F18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J18" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
+      <c r="J18" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="21"/>
       <c r="E19" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>57</v>
+      <c r="F19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J19" s="12" t="s">
-        <v>126</v>
+      <c r="J19" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K19" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="21" t="s">
         <v>77</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>57</v>
+      <c r="F20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J20" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="23"/>
+      <c r="J20" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="21"/>
       <c r="E21" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>57</v>
+      <c r="F21" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I21" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="12" t="s">
-        <v>128</v>
+      <c r="J21" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K21" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
+        <v>127</v>
+      </c>
+      <c r="L21" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="21"/>
       <c r="E22" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="25"/>
-      <c r="G22" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>57</v>
+      <c r="F22" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J22" s="12" t="s">
-        <v>129</v>
+      <c r="J22" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K22" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A23" s="21"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="23" t="s">
+      <c r="D23" s="21" t="s">
         <v>78</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>57</v>
+      <c r="F23" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J23" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
+      <c r="J23" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="25"/>
-      <c r="G24" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>57</v>
+      <c r="F24" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I24" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J24" s="12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="23"/>
+      <c r="J24" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K24" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="21"/>
       <c r="E25" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="25"/>
-      <c r="G25" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>57</v>
+      <c r="F25" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I25" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>132</v>
+      <c r="J25" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K25" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="105" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="23" t="s">
+      <c r="D26" s="21" t="s">
         <v>82</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>57</v>
+      <c r="F26" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I26" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J26" s="13" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A27" s="21"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
+      <c r="J26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="21"/>
       <c r="E27" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="25"/>
-      <c r="G27" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>57</v>
+      <c r="F27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I27" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="12" t="s">
-        <v>134</v>
+      <c r="J27" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K27" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="21"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="23"/>
+        <v>133</v>
+      </c>
+      <c r="L27" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>57</v>
+      <c r="F28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I28" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="12" t="s">
-        <v>135</v>
+      <c r="J28" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K28" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A29" s="21"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="L28" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="23" t="s">
+      <c r="D29" s="21" t="s">
         <v>84</v>
       </c>
       <c r="E29" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F29" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>57</v>
+      <c r="F29" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J29" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="22"/>
-      <c r="D30" s="23"/>
+      <c r="J29" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="21"/>
       <c r="E30" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F30" s="25"/>
-      <c r="G30" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>57</v>
+      <c r="F30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I30" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J30" s="12" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
+      <c r="J30" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K30" s="12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="21"/>
       <c r="E31" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F31" s="25"/>
-      <c r="G31" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>57</v>
+      <c r="F31" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I31" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>138</v>
+      <c r="J31" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="L31" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="D32" s="23" t="s">
+      <c r="D32" s="21" t="s">
         <v>92</v>
       </c>
       <c r="E32" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G32" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>57</v>
+      <c r="F32" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I32" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="23"/>
+      <c r="J32" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="F33" s="25"/>
-      <c r="G33" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>57</v>
+      <c r="F33" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I33" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I34" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K34" s="12" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F34" s="25"/>
-      <c r="G34" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J34" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="120" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="22" t="s">
+      <c r="L34" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="120" x14ac:dyDescent="0.25">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="23" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="23" t="s">
+      <c r="D35" s="21" t="s">
         <v>93</v>
       </c>
       <c r="E35" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G35" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>57</v>
+      <c r="F35" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I35" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="23"/>
+      <c r="J35" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="21"/>
       <c r="E36" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F36" s="25"/>
-      <c r="G36" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>57</v>
+      <c r="F36" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I36" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J36" s="12" t="s">
+      <c r="J36" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K36" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="I37" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K37" s="12" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="21"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="25"/>
-      <c r="G37" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="K37" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22" t="s">
+      <c r="L37" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="D38" s="23" t="s">
+      <c r="D38" s="21" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F38" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>57</v>
+      <c r="F38" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I38" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J38" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A39" s="21"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
+      <c r="J38" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K38" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="21"/>
       <c r="E39" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F39" s="25"/>
-      <c r="G39" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>57</v>
+      <c r="F39" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I39" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="12" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="23"/>
+      <c r="J39" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="21"/>
       <c r="E40" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="25"/>
-      <c r="G40" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>57</v>
+      <c r="F40" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I40" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="12" t="s">
-        <v>147</v>
+      <c r="J40" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K40" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="135" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="L40" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="135" x14ac:dyDescent="0.25">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="D41" s="23" t="s">
+      <c r="D41" s="21" t="s">
         <v>96</v>
       </c>
       <c r="E41" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F41" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>57</v>
+      <c r="F41" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I41" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J41" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A42" s="21"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="22"/>
-      <c r="D42" s="23"/>
+      <c r="J41" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="23"/>
+      <c r="D42" s="21"/>
       <c r="E42" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F42" s="25"/>
-      <c r="G42" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>57</v>
+      <c r="F42" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I42" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J42" s="12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="23"/>
+      <c r="J42" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K42" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="23"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F43" s="25"/>
-      <c r="G43" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>57</v>
+      <c r="F43" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I43" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J43" s="12" t="s">
-        <v>150</v>
+      <c r="J43" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K43" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="180" x14ac:dyDescent="0.25">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="L43" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="180" x14ac:dyDescent="0.25">
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="21" t="s">
         <v>97</v>
       </c>
       <c r="E44" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="F44" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>57</v>
+      <c r="F44" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I44" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J44" s="13" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="21"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="22"/>
-      <c r="D45" s="23"/>
+      <c r="J44" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K44" s="13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="21"/>
       <c r="E45" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F45" s="25"/>
-      <c r="G45" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>57</v>
+      <c r="F45" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I45" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J45" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A46" s="21"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="23"/>
+      <c r="J45" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K45" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="24"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="21"/>
       <c r="E46" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F46" s="25"/>
-      <c r="G46" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>57</v>
+      <c r="F46" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I46" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J46" s="12" t="s">
-        <v>153</v>
+      <c r="J46" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K46" s="12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="120" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="L46" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="D47" s="23" t="s">
+      <c r="D47" s="21" t="s">
         <v>101</v>
       </c>
       <c r="E47" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F47" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>57</v>
+      <c r="F47" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I47" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J47" s="13" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A48" s="21"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="22"/>
-      <c r="D48" s="23"/>
+      <c r="J47" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K47" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="75" x14ac:dyDescent="0.25">
+      <c r="A48" s="24"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="21"/>
       <c r="E48" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="F48" s="25"/>
-      <c r="G48" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>57</v>
+      <c r="F48" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I48" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="12" t="s">
-        <v>154</v>
+      <c r="J48" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K48" s="12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A49" s="21"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="23"/>
+        <v>153</v>
+      </c>
+      <c r="L48" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A49" s="24"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="23"/>
+      <c r="D49" s="21"/>
       <c r="E49" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F49" s="25"/>
-      <c r="G49" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>57</v>
+      <c r="F49" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>176</v>
       </c>
       <c r="I49" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="J49" s="12" t="s">
-        <v>150</v>
+      <c r="J49" s="10" t="s">
+        <v>106</v>
       </c>
       <c r="K49" s="12" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="L49" s="12" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="6"/>
       <c r="D55" s="6"/>
-      <c r="F55" s="8"/>
       <c r="J55" s="8"/>
-    </row>
-    <row r="56" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K55" s="8"/>
+    </row>
+    <row r="56" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B56" s="6"/>
       <c r="D56" s="6"/>
-      <c r="F56" s="8"/>
       <c r="J56" s="8"/>
-    </row>
-    <row r="57" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K56" s="8"/>
+    </row>
+    <row r="57" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="6"/>
       <c r="D57" s="6"/>
-      <c r="F57" s="8"/>
       <c r="J57" s="8"/>
-    </row>
-    <row r="58" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="K57" s="8"/>
+    </row>
+    <row r="58" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="12" t="s">
         <v>8</v>
       </c>
@@ -2574,17 +2792,17 @@
       <c r="E58" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="F58" t="s">
+        <v>41</v>
+      </c>
       <c r="G58" t="s">
-        <v>41</v>
-      </c>
-      <c r="H58" t="s">
         <v>40</v>
       </c>
       <c r="I58" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>8</v>
       </c>
@@ -2600,17 +2818,17 @@
       <c r="E59" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="F59" t="s">
+        <v>41</v>
+      </c>
       <c r="G59" t="s">
-        <v>41</v>
-      </c>
-      <c r="H59" t="s">
         <v>40</v>
       </c>
       <c r="I59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A60" s="12" t="s">
         <v>8</v>
       </c>
@@ -2626,17 +2844,17 @@
       <c r="E60" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="F60" t="s">
+        <v>41</v>
+      </c>
       <c r="G60" t="s">
-        <v>41</v>
-      </c>
-      <c r="H60" t="s">
         <v>40</v>
       </c>
       <c r="I60" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>8</v>
       </c>
@@ -2652,17 +2870,17 @@
       <c r="E61" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="F61" t="s">
+        <v>41</v>
+      </c>
       <c r="G61" t="s">
-        <v>41</v>
-      </c>
-      <c r="H61" t="s">
         <v>40</v>
       </c>
       <c r="I61" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12" t="s">
         <v>8</v>
       </c>
@@ -2678,17 +2896,17 @@
       <c r="E62" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="F62" t="s">
+        <v>41</v>
+      </c>
       <c r="G62" t="s">
-        <v>41</v>
-      </c>
-      <c r="H62" t="s">
         <v>40</v>
       </c>
       <c r="I62" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>8</v>
       </c>
@@ -2704,17 +2922,17 @@
       <c r="E63" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="F63" t="s">
+        <v>41</v>
+      </c>
       <c r="G63" t="s">
-        <v>41</v>
-      </c>
-      <c r="H63" t="s">
         <v>40</v>
       </c>
       <c r="I63" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="12" t="s">
         <v>8</v>
       </c>
@@ -2730,10 +2948,10 @@
       <c r="E64" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="F64" t="s">
+        <v>41</v>
+      </c>
       <c r="G64" t="s">
-        <v>41</v>
-      </c>
-      <c r="H64" t="s">
         <v>40</v>
       </c>
       <c r="I64" t="s">
@@ -2756,10 +2974,10 @@
       <c r="E65" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="F65" t="s">
+        <v>41</v>
+      </c>
       <c r="G65" t="s">
-        <v>41</v>
-      </c>
-      <c r="H65" t="s">
         <v>40</v>
       </c>
       <c r="I65" t="s">
@@ -2782,10 +3000,10 @@
       <c r="E66" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="F66" t="s">
+        <v>41</v>
+      </c>
       <c r="G66" t="s">
-        <v>41</v>
-      </c>
-      <c r="H66" t="s">
         <v>40</v>
       </c>
       <c r="I66" t="s">
@@ -2808,10 +3026,10 @@
       <c r="E67" s="12" t="s">
         <v>44</v>
       </c>
+      <c r="F67" t="s">
+        <v>41</v>
+      </c>
       <c r="G67" t="s">
-        <v>41</v>
-      </c>
-      <c r="H67" t="s">
         <v>40</v>
       </c>
       <c r="I67" t="s">
@@ -2834,10 +3052,10 @@
       <c r="E68" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="F68" t="s">
+        <v>41</v>
+      </c>
       <c r="G68" t="s">
-        <v>41</v>
-      </c>
-      <c r="H68" t="s">
         <v>40</v>
       </c>
       <c r="I68" t="s">
@@ -2860,10 +3078,10 @@
       <c r="E69" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="F69" t="s">
+        <v>41</v>
+      </c>
       <c r="G69" t="s">
-        <v>41</v>
-      </c>
-      <c r="H69" t="s">
         <v>40</v>
       </c>
       <c r="I69" t="s">
@@ -2886,10 +3104,10 @@
       <c r="E70" s="12" t="s">
         <v>45</v>
       </c>
+      <c r="F70" t="s">
+        <v>41</v>
+      </c>
       <c r="G70" t="s">
-        <v>41</v>
-      </c>
-      <c r="H70" t="s">
         <v>40</v>
       </c>
       <c r="I70" t="s">
@@ -2912,10 +3130,10 @@
       <c r="E71" s="12" t="s">
         <v>46</v>
       </c>
+      <c r="F71" t="s">
+        <v>41</v>
+      </c>
       <c r="G71" t="s">
-        <v>41</v>
-      </c>
-      <c r="H71" t="s">
         <v>40</v>
       </c>
       <c r="I71" t="s">
@@ -2938,10 +3156,10 @@
       <c r="E72" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="F72" t="s">
+        <v>41</v>
+      </c>
       <c r="G72" t="s">
-        <v>41</v>
-      </c>
-      <c r="H72" t="s">
         <v>40</v>
       </c>
       <c r="I72" t="s">
@@ -2964,10 +3182,10 @@
       <c r="E73" s="12" t="s">
         <v>50</v>
       </c>
+      <c r="F73" t="s">
+        <v>41</v>
+      </c>
       <c r="G73" t="s">
-        <v>41</v>
-      </c>
-      <c r="H73" t="s">
         <v>40</v>
       </c>
       <c r="I73" t="s">
@@ -2975,43 +3193,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="F47:F49"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="F41:F43"/>
-    <mergeCell ref="F44:F46"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C38:C40"/>
+  <mergeCells count="34">
     <mergeCell ref="B2:B49"/>
     <mergeCell ref="A2:A49"/>
     <mergeCell ref="C17:C19"/>
@@ -3026,6 +3208,26 @@
     <mergeCell ref="C26:C28"/>
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C20:C22"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="D44:D46"/>
+    <mergeCell ref="D47:D49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="D32:D34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3072,20 +3274,20 @@
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18" t="s">
@@ -3102,25 +3304,25 @@
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B6" s="18"/>
       <c r="C6" s="18" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18" t="s">
@@ -3128,27 +3330,27 @@
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -3157,7 +3359,7 @@
       <c r="A10" s="18"/>
       <c r="B10" s="18"/>
       <c r="C10" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
@@ -3175,15 +3377,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFCF9BE3DDC69D46817A851BEC5550B1" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="6f429ff05de3a495de36a912eeee1367">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cbd820e2-9c8a-4c01-9a9c-6b4c26777899" xmlns:ns3="51aa521f-7cbd-47c5-afee-4a8147a04eed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8dba9ee4a9862521e056f2186065b8ec" ns2:_="" ns3:_="">
     <xsd:import namespace="cbd820e2-9c8a-4c01-9a9c-6b4c26777899"/>
@@ -3414,15 +3607,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0813D6E-6704-44BB-86A0-53EB7147135C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E67A2DEA-627F-45CD-8A5E-DEB4B7BB5A7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3439,4 +3633,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E0813D6E-6704-44BB-86A0-53EB7147135C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>